<commit_message>
Use Cases + Scénarios
Rédaction des premiers uses cases et des scénarios
</commit_message>
<xml_diff>
--- a/Journal de travail.xlsx
+++ b/Journal de travail.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="11415"/>
   </bookViews>
   <sheets>
     <sheet name="Agenda" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>DATE</t>
   </si>
@@ -207,6 +207,24 @@
   </si>
   <si>
     <t>Recherches approfondie sur le composant Mathf</t>
+  </si>
+  <si>
+    <t>90 min</t>
+  </si>
+  <si>
+    <t>Réalisation des uses cases</t>
+  </si>
+  <si>
+    <t>60 min</t>
+  </si>
+  <si>
+    <t>15 min</t>
+  </si>
+  <si>
+    <t>Création du repository en ligne</t>
+  </si>
+  <si>
+    <t>Github</t>
   </si>
 </sst>
 </file>
@@ -520,8 +538,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Log" displayName="Log" ref="B2:E36" totalsRowShown="0">
-  <autoFilter ref="B2:E36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Log" displayName="Log" ref="B2:E37" totalsRowShown="0">
+  <autoFilter ref="B2:E37"/>
   <tableColumns count="4">
     <tableColumn id="1" name="DATE" dataCellStyle="Date Column"/>
     <tableColumn id="2" name="HEURE" dataCellStyle="Time Column"/>
@@ -768,10 +786,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E36"/>
+  <dimension ref="B1:E37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -808,8 +826,8 @@
       <c r="B3" s="3">
         <v>43132</v>
       </c>
-      <c r="C3" s="2">
-        <v>0.60416666666666663</v>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>56</v>
@@ -822,8 +840,8 @@
       <c r="B4" s="3">
         <v>43132</v>
       </c>
-      <c r="C4" s="2">
-        <v>0.61111111111111105</v>
+      <c r="C4" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>60</v>
@@ -831,22 +849,34 @@
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="10"/>
+      <c r="B5" s="3">
+        <v>43133</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="6" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>43133</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <v>43136</v>
+        <v>43133</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="4"/>
@@ -854,15 +884,15 @@
     </row>
     <row r="8" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
-        <v>43137</v>
+        <v>43136</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="4"/>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11">
-        <v>43139</v>
+      <c r="B9" s="3">
+        <v>43137</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4"/>
@@ -870,7 +900,7 @@
     </row>
     <row r="10" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="11">
-        <v>43140</v>
+        <v>43139</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="4"/>
@@ -878,7 +908,7 @@
     </row>
     <row r="11" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="11">
-        <v>43143</v>
+        <v>43140</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="4"/>
@@ -886,7 +916,7 @@
     </row>
     <row r="12" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
-        <v>43144</v>
+        <v>43143</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="4"/>
@@ -894,7 +924,7 @@
     </row>
     <row r="13" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
-        <v>43146</v>
+        <v>43144</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="4"/>
@@ -902,7 +932,7 @@
     </row>
     <row r="14" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
-        <v>43147</v>
+        <v>43146</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="4"/>
@@ -910,7 +940,7 @@
     </row>
     <row r="15" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
-        <v>43157</v>
+        <v>43147</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="4"/>
@@ -918,7 +948,7 @@
     </row>
     <row r="16" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
-        <v>43158</v>
+        <v>43157</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="4"/>
@@ -926,7 +956,7 @@
     </row>
     <row r="17" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
-        <v>371878</v>
+        <v>43158</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="4"/>
@@ -934,7 +964,7 @@
     </row>
     <row r="18" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
-        <v>43161</v>
+        <v>371878</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="4"/>
@@ -942,7 +972,7 @@
     </row>
     <row r="19" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
-        <v>43164</v>
+        <v>43161</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="4"/>
@@ -950,7 +980,7 @@
     </row>
     <row r="20" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
-        <v>43165</v>
+        <v>43164</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="4"/>
@@ -958,7 +988,7 @@
     </row>
     <row r="21" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
-        <v>43167</v>
+        <v>43165</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="4"/>
@@ -966,7 +996,7 @@
     </row>
     <row r="22" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
-        <v>43168</v>
+        <v>43167</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="4"/>
@@ -974,7 +1004,7 @@
     </row>
     <row r="23" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
-        <v>43171</v>
+        <v>43168</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="4"/>
@@ -982,7 +1012,7 @@
     </row>
     <row r="24" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
-        <v>43172</v>
+        <v>43171</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="4"/>
@@ -990,7 +1020,7 @@
     </row>
     <row r="25" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
-        <v>43174</v>
+        <v>43172</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="4"/>
@@ -998,7 +1028,7 @@
     </row>
     <row r="26" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
-        <v>43175</v>
+        <v>43174</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="4"/>
@@ -1006,7 +1036,7 @@
     </row>
     <row r="27" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
-        <v>43178</v>
+        <v>43175</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="4"/>
@@ -1014,7 +1044,7 @@
     </row>
     <row r="28" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="11">
-        <v>43179</v>
+        <v>43178</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="4"/>
@@ -1022,7 +1052,7 @@
     </row>
     <row r="29" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11">
-        <v>43181</v>
+        <v>43179</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="4"/>
@@ -1030,7 +1060,7 @@
     </row>
     <row r="30" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="11">
-        <v>43185</v>
+        <v>43181</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="4"/>
@@ -1038,7 +1068,7 @@
     </row>
     <row r="31" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11">
-        <v>43186</v>
+        <v>43185</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="4"/>
@@ -1046,7 +1076,7 @@
     </row>
     <row r="32" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11">
-        <v>43188</v>
+        <v>43186</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="4"/>
@@ -1054,7 +1084,7 @@
     </row>
     <row r="33" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="11">
-        <v>43206</v>
+        <v>43188</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="4"/>
@@ -1062,7 +1092,7 @@
     </row>
     <row r="34" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="11">
-        <v>43207</v>
+        <v>43206</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="4"/>
@@ -1070,7 +1100,7 @@
     </row>
     <row r="35" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="11">
-        <v>43209</v>
+        <v>43207</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="4"/>
@@ -1078,11 +1108,19 @@
     </row>
     <row r="36" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="11">
-        <v>43210</v>
+        <v>43209</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="4"/>
       <c r="E36" s="10"/>
+    </row>
+    <row r="37" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="11">
+        <v>43210</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="10"/>
     </row>
   </sheetData>
   <dataValidations xWindow="45" yWindow="267" count="5">
@@ -1409,6 +1447,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1589,27 +1647,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1626,22 +1682,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
06.02.2018 -  réalisation des maquettes
Réalisation des maquettes du menu principal et du menu d'édition
</commit_message>
<xml_diff>
--- a/Journal de travail.xlsx
+++ b/Journal de travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t>DATE</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>changement dans certains uses cases et insertion de divers scenarios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réalisation des maquettes ( menu principal, menu d'édition) </t>
   </si>
 </sst>
 </file>
@@ -795,7 +798,7 @@
   <dimension ref="B1:E36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -898,8 +901,12 @@
       <c r="B8" s="3">
         <v>43137</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="2:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1460,6 +1467,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AA3F7D94069FF64A86F7DFF56D60E3BE" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c32302c77d4085ecf495bdddb7f5e889">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a4f35948-e619-41b3-aa29-22878b09cfd2" xmlns:ns3="40262f94-9f35-4ac3-9a90-690165a166b7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4ab5ae46be95f9d0be6107e8200be7a2" ns2:_="" ns3:_="">
     <xsd:import namespace="a4f35948-e619-41b3-aa29-22878b09cfd2"/>
@@ -1640,17 +1658,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <VSO_x0020_item_x0020_id xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Assetid_x0020_ xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Item_x0020_Details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-    <Template_x0020_details xmlns="40262f94-9f35-4ac3-9a90-690165a166b7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1934E82E-1C0E-415F-9886-064BC72C3B49}">
   <ds:schemaRefs>
@@ -1660,6 +1667,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B53890C6-895E-4346-BCB4-738C50EDC5D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1676,14 +1693,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{885137DC-D143-4691-87B9-2812AFF1A34F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="40262f94-9f35-4ac3-9a90-690165a166b7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>